<commit_message>
v.4 delete after method and before method and solved wait problem in title
</commit_message>
<xml_diff>
--- a/files/conduittests/login/LoginTest.xlsx
+++ b/files/conduittests/login/LoginTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\conduittests\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DC034F-4DD6-4627-BD0D-7B88112DA8A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14B2F6D-2654-4CED-A3A3-B3B6FF945CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DF7C5555-2B13-40D0-92BE-E3AAA4F1FB06}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,8 +489,12 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>12345678</v>
+      </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
@@ -541,12 +545,8 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
-        <v>12345678</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" t="s">
         <v>13</v>
       </c>
@@ -561,7 +561,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +604,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>123456789</v>
+        <v>12345678955</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1">
-        <v>12345678910</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1">
-        <v>12345678910</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1">
-        <v>12345678910</v>
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parent class, but tests are not completed
</commit_message>
<xml_diff>
--- a/files/conduittests/login/LoginTest.xlsx
+++ b/files/conduittests/login/LoginTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\conduittests\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14B2F6D-2654-4CED-A3A3-B3B6FF945CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE14375-D2D2-41B3-848B-57988C427963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DF7C5555-2B13-40D0-92BE-E3AAA4F1FB06}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,9 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>123456789</v>
+      </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
@@ -604,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>12345678955</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>